<commit_message>
add and assign the testing modules to the team members
</commit_message>
<xml_diff>
--- a/Plans/Lhub_RACI.xlsx
+++ b/Plans/Lhub_RACI.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="63">
   <si>
     <r>
       <t xml:space="preserve">Mohamed Ragab
@@ -200,12 +200,66 @@
   <si>
     <t>Design the Entity Relationship Diagram (ERD)(Lhub_ERD)</t>
   </si>
+  <si>
+    <t>2.4.3  Homepage Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.4.4 Category Module </t>
+  </si>
+  <si>
+    <r>
+      <t>2.4.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>       Login Module</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.4.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>       Registration Module</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.4.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>   Review Articles Module</t>
+    </r>
+  </si>
+  <si>
+    <t>Week 4 (testing phase accoding to SRS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the person who has "C" role will review the work of the  "R" person </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -265,6 +319,19 @@
     </font>
     <font>
       <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -382,21 +449,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -518,8 +583,11 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -815,9 +883,9 @@
   </sheetPr>
   <dimension ref="A1:AB1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1648,91 +1716,160 @@
       <c r="G31" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H31" s="41"/>
+      <c r="H31" s="40"/>
       <c r="I31" s="29"/>
       <c r="J31" s="29"/>
     </row>
-    <row r="32" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-    </row>
-    <row r="33" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+    <row r="32" spans="1:11" s="28" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H33" s="40"/>
       <c r="I33" s="29"/>
       <c r="J33" s="29"/>
-    </row>
-    <row r="34" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
+      <c r="K33" s="41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="40"/>
       <c r="I34" s="29"/>
       <c r="J34" s="29"/>
-    </row>
-    <row r="35" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="K34" s="42"/>
+    </row>
+    <row r="35" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="40"/>
       <c r="I35" s="29"/>
       <c r="J35" s="29"/>
-    </row>
-    <row r="36" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
+      <c r="K35" s="42"/>
+    </row>
+    <row r="36" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" s="40"/>
       <c r="I36" s="29"/>
       <c r="J36" s="29"/>
-    </row>
-    <row r="37" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
+      <c r="K36" s="42"/>
+    </row>
+    <row r="37" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="40"/>
       <c r="I37" s="29"/>
       <c r="J37" s="29"/>
-    </row>
-    <row r="38" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="K37" s="42"/>
+    </row>
+    <row r="38" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="30"/>
+      <c r="H38" s="40"/>
       <c r="I38" s="29"/>
       <c r="J38" s="29"/>
     </row>
-    <row r="39" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30"/>
+      <c r="H39" s="40"/>
       <c r="I39" s="29"/>
       <c r="J39" s="29"/>
     </row>
-    <row r="40" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="30"/>
+      <c r="H40" s="40"/>
       <c r="I40" s="29"/>
       <c r="J40" s="29"/>
     </row>
-    <row r="41" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="30"/>
+      <c r="H41" s="40"/>
       <c r="I41" s="29"/>
       <c r="J41" s="29"/>
     </row>
-    <row r="42" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
+      <c r="H42" s="40"/>
       <c r="I42" s="29"/>
       <c r="J42" s="29"/>
     </row>
-    <row r="43" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30"/>
+      <c r="H43" s="40"/>
       <c r="I43" s="29"/>
       <c r="J43" s="29"/>
     </row>
-    <row r="44" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="30"/>
+      <c r="H44" s="40"/>
       <c r="I44" s="29"/>
       <c r="J44" s="29"/>
     </row>
-    <row r="45" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
       <c r="I45" s="29"/>
       <c r="J45" s="29"/>
     </row>
-    <row r="46" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="30"/>
       <c r="I46" s="29"/>
       <c r="J46" s="29"/>
     </row>
-    <row r="47" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="30"/>
       <c r="I47" s="29"/>
       <c r="J47" s="29"/>
     </row>
-    <row r="48" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="30"/>
       <c r="I48" s="29"/>
       <c r="J48" s="29"/>
@@ -6508,9 +6645,10 @@
       <c r="J1002" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="H1:H13"/>
-    <mergeCell ref="H14:H31"/>
+    <mergeCell ref="H14:H44"/>
+    <mergeCell ref="K33:K37"/>
   </mergeCells>
   <conditionalFormatting sqref="G11">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="A">

</xml_diff>